<commit_message>
Resolves: #1 Fix formulas for displayed calendar stats
The formulas for the summmary statistics (# days, # weekdays,
were incorrect.

In addition, a warning message has been added if the calendar range
represented by the specified Start Date and End Date would not fit
in the 12-week display area.
</commit_message>
<xml_diff>
--- a/On Call Calendar.xlsx
+++ b/On Call Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shlomo/git_repos/on-call-calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0843D8B-4D43-314B-B352-777757DD9AB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D202EDB8-6293-D142-8F0F-0FEE005842B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{C3BD2156-5360-E34F-B527-DDC5436CA037}"/>
   </bookViews>
@@ -173,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -195,6 +195,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -216,14 +219,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -233,21 +229,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u val="double"/>
-        <color rgb="FFC00000"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -263,116 +244,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u val="double"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u val="double"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u val="double"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -419,16 +290,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9373426-1796-304B-A226-49AAED9D8823}" name="Table1" displayName="Table1" ref="J8:L13" totalsRowShown="0" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9373426-1796-304B-A226-49AAED9D8823}" name="Table1" displayName="Table1" ref="J8:L13" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="J8:L13" xr:uid="{F38F8A8C-7A74-4A48-AFCB-C2B997FC24D2}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5B6C6BD1-0CE4-7C43-8CAC-AF9461F5F7DD}" name="Date" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{C6E87BE1-5E41-1149-8813-DB59EBAA5168}" name="Description" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{68FC5954-1CA7-EC46-AE34-B2B26B13AF52}" name="Assignment" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{5B6C6BD1-0CE4-7C43-8CAC-AF9461F5F7DD}" name="Date" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C6E87BE1-5E41-1149-8813-DB59EBAA5168}" name="Description" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{68FC5954-1CA7-EC46-AE34-B2B26B13AF52}" name="Assignment" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -734,7 +605,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,22 +628,22 @@
         <v>0</v>
       </c>
       <c r="C3" s="8">
-        <v>43972</v>
-      </c>
-      <c r="D3" s="15" t="s">
+        <v>43971</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="16"/>
       <c r="F3" s="4">
-        <f>C4-C3</f>
-        <v>76</v>
+        <f>C4-C3+1</f>
+        <v>80</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H3" t="str">
-        <f>INDEX($B$8:$H$8,WEEKDAY($C3,1))</f>
-        <v>Thursday</v>
+        <f>INDEX($B$8:$H$8,WEEKDAY($C3))</f>
+        <v>Wednesday</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -780,58 +651,64 @@
         <v>1</v>
       </c>
       <c r="C4" s="8">
-        <v>44048</v>
-      </c>
-      <c r="D4" s="15" t="s">
+        <v>44050</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="4">
-        <f>F3-F5</f>
-        <v>54</v>
+        <f ca="1">F3-F5</f>
+        <v>58</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H4" t="str">
-        <f>INDEX($B$8:$H$8,WEEKDAY($C4,1))</f>
-        <v>Wednesday</v>
-      </c>
+        <f>INDEX($B$8:$H$8,WEEKDAY($C4))</f>
+        <v>Friday</v>
+      </c>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D5" s="15" t="s">
+      <c r="B5" t="str">
+        <f>IF(C4-C3&gt;84-WEEKDAY(C3),"Beyond a 12 week calendar","")</f>
+        <v/>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="6">
-        <f>INT((WEEKDAY(C3-2)-C3+C4)/7)+INT((WEEKDAY(C3-4)-C3+C4)/7)</f>
+        <f ca="1">SUMPRODUCT((WEEKDAY(ROW(INDIRECT(C3&amp;":"&amp;C4)))={1,7})*1)</f>
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="15"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="6">
-        <f>COUNTIFS(Table1[Date],"&gt;="&amp;$C$3,Table1[Date],"&lt;="&amp;$C$4)</f>
+        <f>SUMPRODUCT(1*(Table1[Date]&gt;=C3)*(Table1[Date]&lt;=C4)*(WEEKDAY(Table1[Date])&gt;1)*(WEEKDAY(Table1[Date])&lt;7))</f>
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H6" t="str">
-        <f>INT((F3+1)/7)&amp;" + "&amp;MOD(F3+1,7)&amp;" day"&amp;IF(MOD(F3+1,7)&lt;&gt;1,"s","")</f>
-        <v>11 + 0 days</v>
-      </c>
+        <f>INT(F3/7)&amp;" + "&amp;MOD(F3,7)&amp;" day"&amp;IF(MOD(F3,7)&lt;&gt;1,"s","")</f>
+        <v>11 + 3 days</v>
+      </c>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
@@ -869,36 +746,36 @@
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B9" s="11" t="str">
+      <c r="B9" s="12" t="str">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v/>
       </c>
-      <c r="C9" s="11" t="str">
+      <c r="C9" s="12" t="str">
         <f t="shared" ref="C9:H31" si="0">IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v/>
       </c>
-      <c r="D9" s="11" t="str">
+      <c r="D9" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E9" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F9" s="11">
+      <c r="E9" s="12">
+        <f t="shared" si="0"/>
+        <v>43971</v>
+      </c>
+      <c r="F9" s="12">
         <f t="shared" si="0"/>
         <v>43972</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="12">
         <f t="shared" si="0"/>
         <v>43973</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="12">
         <f t="shared" si="0"/>
         <v>43974</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="13">
+      <c r="J9" s="14">
         <v>43976</v>
       </c>
       <c r="K9" s="9" t="s">
@@ -912,14 +789,14 @@
       <c r="T9" s="3"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="J10" s="13">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="J10" s="14">
         <v>44074</v>
       </c>
       <c r="K10" s="9" t="s">
@@ -928,36 +805,36 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="11">
+      <c r="B11" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>43975</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="12">
         <f t="shared" si="0"/>
         <v>43976</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>43977</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="12">
         <f t="shared" si="0"/>
         <v>43978</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="12">
         <f t="shared" si="0"/>
         <v>43979</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="12">
         <f t="shared" si="0"/>
         <v>43980</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="12">
         <f t="shared" si="0"/>
         <v>43981</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="13">
+      <c r="J11" s="14">
         <v>44161</v>
       </c>
       <c r="K11" s="9" t="s">
@@ -966,16 +843,16 @@
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="J12" s="13">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="J12" s="14">
         <v>44190</v>
       </c>
       <c r="K12" s="9" t="s">
@@ -984,36 +861,36 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="11">
+      <c r="B13" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>43982</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="12">
         <f t="shared" si="0"/>
         <v>43983</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
         <v>43984</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="12">
         <f t="shared" si="0"/>
         <v>43985</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="12">
         <f t="shared" si="0"/>
         <v>43986</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="12">
         <f t="shared" si="0"/>
         <v>43987</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="12">
         <f t="shared" si="0"/>
         <v>43988</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="13">
+      <c r="J13" s="14">
         <v>44196</v>
       </c>
       <c r="K13" s="9" t="s">
@@ -1022,370 +899,370 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B15" s="11">
+      <c r="B15" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>43989</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="12">
         <f t="shared" si="0"/>
         <v>43990</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="12">
         <f t="shared" si="0"/>
         <v>43991</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="12">
         <f t="shared" si="0"/>
         <v>43992</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="12">
         <f t="shared" si="0"/>
         <v>43993</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="12">
         <f t="shared" si="0"/>
         <v>43994</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="12">
         <f t="shared" si="0"/>
         <v>43995</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="11">
+      <c r="B17" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>43996</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="12">
         <f t="shared" si="0"/>
         <v>43997</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="12">
         <f t="shared" si="0"/>
         <v>43998</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="12">
         <f t="shared" si="0"/>
         <v>43999</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="12">
         <f t="shared" si="0"/>
         <v>44000</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="12">
         <f t="shared" si="0"/>
         <v>44001</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="12">
         <f t="shared" si="0"/>
         <v>44002</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="11">
+      <c r="B19" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>44003</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="12">
         <f t="shared" si="0"/>
         <v>44004</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="12">
         <f t="shared" si="0"/>
         <v>44005</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="12">
         <f t="shared" si="0"/>
         <v>44006</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="12">
         <f t="shared" si="0"/>
         <v>44007</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="12">
         <f t="shared" si="0"/>
         <v>44008</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="12">
         <f t="shared" si="0"/>
         <v>44009</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="11">
+      <c r="B21" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>44010</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="12">
         <f t="shared" si="0"/>
         <v>44011</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="12">
         <f t="shared" si="0"/>
         <v>44012</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="12">
         <f t="shared" si="0"/>
         <v>44013</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="12">
         <f t="shared" si="0"/>
         <v>44014</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="12">
         <f t="shared" si="0"/>
         <v>44015</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="12">
         <f t="shared" si="0"/>
         <v>44016</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="11">
+      <c r="B23" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>44017</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="12">
         <f t="shared" si="0"/>
         <v>44018</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="12">
         <f t="shared" si="0"/>
         <v>44019</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="12">
         <f t="shared" si="0"/>
         <v>44020</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="12">
         <f t="shared" si="0"/>
         <v>44021</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="12">
         <f t="shared" si="0"/>
         <v>44022</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="12">
         <f t="shared" si="0"/>
         <v>44023</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="11">
+      <c r="B25" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>44024</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="12">
         <f t="shared" si="0"/>
         <v>44025</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="12">
         <f t="shared" si="0"/>
         <v>44026</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="12">
         <f t="shared" si="0"/>
         <v>44027</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="12">
         <f t="shared" si="0"/>
         <v>44028</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="12">
         <f t="shared" si="0"/>
         <v>44029</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="12">
         <f t="shared" si="0"/>
         <v>44030</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="11">
+      <c r="B27" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>44031</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="12">
         <f t="shared" si="0"/>
         <v>44032</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="12">
         <f t="shared" si="0"/>
         <v>44033</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="12">
         <f t="shared" si="0"/>
         <v>44034</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="12">
         <f t="shared" si="0"/>
         <v>44035</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="12">
         <f t="shared" si="0"/>
         <v>44036</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="12">
         <f t="shared" si="0"/>
         <v>44037</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="11">
+      <c r="B29" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>44038</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="12">
         <f t="shared" si="0"/>
         <v>44039</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="12">
         <f t="shared" si="0"/>
         <v>44040</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="12">
         <f t="shared" si="0"/>
         <v>44041</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="12">
         <f t="shared" si="0"/>
         <v>44042</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="12">
         <f t="shared" si="0"/>
         <v>44043</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="12">
         <f t="shared" si="0"/>
         <v>44044</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="11">
+      <c r="B31" s="12">
         <f>IF(AND(7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&gt;=$C$3,7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9)&lt;=$C$4),7*INT((ROW()-ROW($B$9))/2)+$C$3-WEEKDAY($C$3+1,3)+COLUMN()-COLUMN($B$9),"")</f>
         <v>44045</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="12">
         <f t="shared" si="0"/>
         <v>44046</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="12">
         <f t="shared" si="0"/>
         <v>44047</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="12">
         <f t="shared" si="0"/>
         <v>44048</v>
       </c>
-      <c r="F31" s="11" t="str">
+      <c r="F31" s="12">
+        <f t="shared" si="0"/>
+        <v>44049</v>
+      </c>
+      <c r="G31" s="12">
+        <f t="shared" si="0"/>
+        <v>44050</v>
+      </c>
+      <c r="H31" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G31" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H31" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -1397,17 +1274,22 @@
     <mergeCell ref="D6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:H32">
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="4" priority="13">
       <formula>N("Date cell for holidays")+AND(MOD(ROW()-ROW($B$9),2)=0,B9&lt;&gt;"",NOT(ISERROR(MATCH(B9,$J$9:$J$22,0))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="14">
+    <cfRule type="expression" dxfId="3" priority="15">
       <formula>N("Cells outside the calendar range")+OR(AND(MOD(ROW()-ROW($B$9),2)=0,B9=""),AND(MOD(ROW()-ROW($B$9),2)=1,B8="",B9=""))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="15">
+    <cfRule type="expression" dxfId="2" priority="16">
       <formula>N("Assigment cell that differs from holiday assignment table entry")+AND(MOD(ROW()-ROW($B$9),2)=1,IF(NOT(ISNA(MATCH(B8,$J$9:$J$24,0))),INDEX($L$9:$L$24,MATCH(B8,$J$9:$J$24,0))&lt;&gt;B9,FALSE))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="16">
+    <cfRule type="expression" dxfId="1" priority="17">
       <formula>N("Assignment cell that is filled")+AND(MOD(ROW()-ROW($B$9),2)=1,B8&lt;&gt;"",B9&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4 B5:C5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>LEN($B$5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: One conditional formatting rule for an assigned day
The conditional formatting rule for assigned days used to only format
the assignment cell, not the date cell. This change makes it also format
the date cell.
</commit_message>
<xml_diff>
--- a/On Call Calendar.xlsx
+++ b/On Call Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shlomo/git_repos/on-call-calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D202EDB8-6293-D142-8F0F-0FEE005842B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916B6CDC-2253-4244-9811-F448FCCB9BC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{C3BD2156-5360-E34F-B527-DDC5436CA037}"/>
   </bookViews>
@@ -219,7 +219,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -234,6 +234,48 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u val="double"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -290,16 +332,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9373426-1796-304B-A226-49AAED9D8823}" name="Table1" displayName="Table1" ref="J8:L13" totalsRowShown="0" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9373426-1796-304B-A226-49AAED9D8823}" name="Table1" displayName="Table1" ref="J8:L13" totalsRowShown="0" dataDxfId="13">
   <autoFilter ref="J8:L13" xr:uid="{F38F8A8C-7A74-4A48-AFCB-C2B997FC24D2}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5B6C6BD1-0CE4-7C43-8CAC-AF9461F5F7DD}" name="Date" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{C6E87BE1-5E41-1149-8813-DB59EBAA5168}" name="Description" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{68FC5954-1CA7-EC46-AE34-B2B26B13AF52}" name="Assignment" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{5B6C6BD1-0CE4-7C43-8CAC-AF9461F5F7DD}" name="Date" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{C6E87BE1-5E41-1149-8813-DB59EBAA5168}" name="Description" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{68FC5954-1CA7-EC46-AE34-B2B26B13AF52}" name="Assignment" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1274,21 +1316,21 @@
     <mergeCell ref="D6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:H32">
-    <cfRule type="expression" dxfId="4" priority="13">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>N("Date cell for holidays")+AND(MOD(ROW()-ROW($B$9),2)=0,B9&lt;&gt;"",NOT(ISERROR(MATCH(B9,$J$9:$J$22,0))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="15">
+    <cfRule type="expression" dxfId="8" priority="15">
       <formula>N("Cells outside the calendar range")+OR(AND(MOD(ROW()-ROW($B$9),2)=0,B9=""),AND(MOD(ROW()-ROW($B$9),2)=1,B8="",B9=""))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="16">
+    <cfRule type="expression" dxfId="7" priority="16">
       <formula>N("Assigment cell that differs from holiday assignment table entry")+AND(MOD(ROW()-ROW($B$9),2)=1,IF(NOT(ISNA(MATCH(B8,$J$9:$J$24,0))),INDEX($L$9:$L$24,MATCH(B8,$J$9:$J$24,0))&lt;&gt;B9,FALSE))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17">
-      <formula>N("Assignment cell that is filled")+AND(MOD(ROW()-ROW($B$9),2)=1,B8&lt;&gt;"",B9&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="5" priority="17">
+      <formula>N("Assignment cell that is filled")+OR(AND(MOD(ROW()-ROW($B$8),2)=0,B9&lt;&gt;""),AND(MOD(ROW()-ROW($B$8),2)=1,B10&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4 B5:C5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>LEN($B$5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix: restore comment in conditional formatting
</commit_message>
<xml_diff>
--- a/On Call Calendar.xlsx
+++ b/On Call Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shlomo/git_repos/on-call-calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916B6CDC-2253-4244-9811-F448FCCB9BC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D134E59-8655-5242-838F-FA8388C95CEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{C3BD2156-5360-E34F-B527-DDC5436CA037}"/>
   </bookViews>
@@ -263,19 +263,19 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1325,13 +1325,13 @@
     <cfRule type="expression" dxfId="7" priority="16">
       <formula>N("Assigment cell that differs from holiday assignment table entry")+AND(MOD(ROW()-ROW($B$9),2)=1,IF(NOT(ISNA(MATCH(B8,$J$9:$J$24,0))),INDEX($L$9:$L$24,MATCH(B8,$J$9:$J$24,0))&lt;&gt;B9,FALSE))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="17">
+    <cfRule type="expression" dxfId="6" priority="17">
       <formula>N("Assignment cell that is filled")+OR(AND(MOD(ROW()-ROW($B$8),2)=0,B9&lt;&gt;""),AND(MOD(ROW()-ROW($B$8),2)=1,B10&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4 B5:C5">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>LEN($B$5)&gt;0</formula>
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>N("Date range exceeds 12 displayed weeks")+LEN($B$5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>